<commit_message>
README additions and script cleanup
</commit_message>
<xml_diff>
--- a/data_files/clus_impt_pos.xlsx
+++ b/data_files/clus_impt_pos.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirbyleo/Box Sync/Depot - dDAVP-time course - Kirby/Scripts/time_course_bayes/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirbyleo/Box/Depot - dDAVP-time course - Kirby/Scripts/FinalDirectory/time_course_bayes/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEFB47C2-BC74-3942-B75D-AE03EA60A576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E49C066-2BDC-2A47-ADCD-6F7A4D9DAA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0B4075E2-3BF9-49FF-8BD9-11BFF272F07F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{0B4075E2-3BF9-49FF-8BD9-11BFF272F07F}"/>
   </bookViews>
   <sheets>
-    <sheet name="positioning" sheetId="3" r:id="rId1"/>
+    <sheet name="README" sheetId="4" r:id="rId1"/>
+    <sheet name="positioning" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>IA1</t>
   </si>
@@ -75,6 +76,9 @@
   </si>
   <si>
     <t>IVB</t>
+  </si>
+  <si>
+    <t>The following template ("positioning") is a binary basis on the positions of the high frequency amino acids pinpointed during the initial clustering stages, e.g. +1 for Group I, -3 and -2 for Group II.A. This data is used in the "selectpos_bayes" function in bayesian_module.py</t>
   </si>
 </sst>
 </file>
@@ -132,10 +136,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,10 +457,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE672639-24A1-9A46-8B19-54C7B28A556C}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99A55F4-D959-E74E-9D45-06AA896A4240}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>